<commit_message>
added requirements in matlab
</commit_message>
<xml_diff>
--- a/req/RequiermentsKlimaAnlage.xlsx
+++ b/req/RequiermentsKlimaAnlage.xlsx
@@ -1,68 +1,432 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28224"/>
-  <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97A1E841-F586-4EBF-9FF7-B1867DB17124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kilia\Desktop\UNI\Matlab\Modellbasierte Entwicklung\KlimaAnlage\req\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C769A8FF-F5EE-4F65-AD77-7418046EDE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="RequiermentsKlimaAnlage" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Requierments Klimaanlage</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Kundenanfoderungen</t>
+  </si>
+  <si>
+    <t>relationID</t>
+  </si>
+  <si>
+    <t>ParentID</t>
+  </si>
+  <si>
+    <t>ID_SW</t>
+  </si>
+  <si>
+    <t>Software Anfoderungen Abgeleitet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Klimaanlage muss in der Lage sein, die Innenraumtemperatur in einem Bereich von 
+16°C bis 28°C zu regeln. </t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>Die Klimaanlagensteuerung muss die Temperatur auf eine voreingestellte Zieltemperatur 
+zwischen 16°C und 28°C regeln können.</t>
+  </si>
+  <si>
+    <t>Die Klimaanlage muss bei allen üblichen Außentemperaturen zwischen 
+-20°C und +50°C zuverlässig funktionieren.</t>
+  </si>
+  <si>
+    <t>Die Software muss die Klimaanlage so steuern, dass sie die Innenraumtemperatur in 
+maximal 5 Minuten um mindestens 10°C herunterkühlt oder aufheizen kann.</t>
+  </si>
+  <si>
+    <t>Die Klimaanlage soll das Fahrzeug innerhalb von 5 Minuten auf eine angenehme Temperatur 
+herunterkühlen oder aufheizen.</t>
+  </si>
+  <si>
+    <t>Die Software muss die Innenraumtemperatur auf ±1°C der eingestellten Zieltemperatur 
+halten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Temperatur im Fahrzeuginnenraum soll konstant gehalten werden und Schwankungen
+ von ±1°C nicht überschreiten. </t>
+  </si>
+  <si>
+    <t>3, 4</t>
+  </si>
+  <si>
+    <t>Die Klimaanlage muss basierend auf der Innenraum- und Außentemperatur selbständig 
+die Innenraumtemperatur auf den vom Nutzer eingestellten Sollwert regeln. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Klimaanlage soll einen Automatikmodus besitzen, der selbstständig die ideale 
+Temperatur auf Innen- und Außentemperatur regelt. </t>
+  </si>
+  <si>
+    <t>Die Software muss eine Fehlererkennungsfunktion implementieren, die bei einem Außentemperaturen ab -20°C und  niedriger, sowie +50°C und höher einen Sicherheitsmodus aktiviert. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bei einem Defekt oder einem ungewöhnlich hohen Energieverbrauch soll die Klimaanlage 
+in einen sicheren Modus wechseln, der keine weiteren Schäden verursacht und einen Hinweis im Fahrzeugdisplay gibt. </t>
+  </si>
+  <si>
+    <t>Die Software muss eine Fehlererkennungsfunktion implementieren, die bei einem Energieverbrauch größer als 5kW einen Sicherheitsmodus aktiviert. </t>
+  </si>
+  <si>
+    <t>Im Sicherheitsmodus muss die Klimaanlage deaktiviert werden bis der Energieverbrauch wieder unter 5kW und die Temperatur wieder über -20°C oder unter 50°C beträgt.</t>
+  </si>
+  <si>
+    <t>Eine Meldung „Klimaanlage im Sicherheitsmodus“ muss im Fahrzeugdisplay erscheinen, 
+wenn der Sicherheitsmodus aktiviert ist</t>
+  </si>
+  <si>
+    <t>Die Temperatur muss in 1°C Schritten zwischen 16°C und 28°C vom Nutzer am Bedienelement der Klimaanlagensteuerung eingestellt werden können.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="24"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial Black"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -70,19 +434,210 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -95,7 +650,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -105,39 +660,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="145F82"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E87331"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="186C24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -189,7 +744,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -300,6 +855,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -308,13 +870,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -379,27 +934,7 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
@@ -410,27 +945,210 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:8" ht="36.75">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>1.2</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>